<commit_message>
measure_results all but the wins calculation
</commit_message>
<xml_diff>
--- a/archive/2024/results.xlsx
+++ b/archive/2024/results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Index</t>
   </si>
@@ -55,25 +55,7 @@
     <t>Totals</t>
   </si>
   <si>
-    <t>25%</t>
-  </si>
-  <si>
-    <t>3%</t>
-  </si>
-  <si>
-    <t>6%</t>
-  </si>
-  <si>
-    <t>12%</t>
-  </si>
-  <si>
-    <t>50%</t>
-  </si>
-  <si>
     <t>100%</t>
-  </si>
-  <si>
-    <t>10%</t>
   </si>
 </sst>
 </file>
@@ -465,7 +447,7 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -482,10 +464,10 @@
         <v>32</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -499,10 +481,10 @@
         <v>16</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -516,10 +498,10 @@
         <v>8</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -533,7 +515,7 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -550,10 +532,10 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -570,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -584,10 +566,10 @@
         <v>67</v>
       </c>
       <c r="D9">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
measure_results all but copying bracket and predict to archive directory
</commit_message>
<xml_diff>
--- a/archive/2024/results.xlsx
+++ b/archive/2024/results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Index</t>
   </si>
@@ -55,7 +55,25 @@
     <t>Totals</t>
   </si>
   <si>
+    <t>75%</t>
+  </si>
+  <si>
+    <t>62%</t>
+  </si>
+  <si>
+    <t>69%</t>
+  </si>
+  <si>
+    <t>38%</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
     <t>100%</t>
+  </si>
+  <si>
+    <t>61%</t>
   </si>
 </sst>
 </file>
@@ -447,7 +465,7 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -464,10 +482,10 @@
         <v>32</v>
       </c>
       <c r="D3">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -481,10 +499,10 @@
         <v>16</v>
       </c>
       <c r="D4">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -498,10 +516,10 @@
         <v>8</v>
       </c>
       <c r="D5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -515,10 +533,10 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -532,10 +550,10 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -552,7 +570,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -566,10 +584,10 @@
         <v>67</v>
       </c>
       <c r="D9">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>